<commit_message>
manual data processing updates
</commit_message>
<xml_diff>
--- a/data/timeseries/raw/metrinet-calibration-records.xlsx
+++ b/data/timeseries/raw/metrinet-calibration-records.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\bradw\workspace\bayesian-wq-calibration\data\timeseries\raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEB9167F-6172-4D3D-9C9A-3DB15DF02B3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6049C363-59B9-44F1-B0F8-026619562E65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1305" yWindow="2880" windowWidth="25605" windowHeight="16380" xr2:uid="{5BB3812C-8BE3-4C2C-92EC-D761C3FFAE3F}"/>
+    <workbookView xWindow="2685" yWindow="4260" windowWidth="25605" windowHeight="16380" xr2:uid="{5BB3812C-8BE3-4C2C-92EC-D761C3FFAE3F}"/>
   </bookViews>
   <sheets>
     <sheet name="metrinet_calibration_records(Sh" sheetId="1" r:id="rId1"/>
@@ -1261,8 +1261,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F541CF5D-C4E9-4800-B227-EFCE7BC313D7}">
   <dimension ref="A1:K252"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="O34" sqref="O34"/>
+    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="D89" sqref="D89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2858,7 +2858,7 @@
         <v>44853.415277777778</v>
       </c>
       <c r="D46" s="1">
-        <v>44860</v>
+        <v>44861</v>
       </c>
       <c r="E46">
         <v>0.61</v>
@@ -2893,7 +2893,7 @@
         <v>44853.415277777778</v>
       </c>
       <c r="D47" s="1">
-        <v>44860</v>
+        <v>44861</v>
       </c>
       <c r="E47">
         <v>0.56000000000000005</v>
@@ -2928,7 +2928,7 @@
         <v>44853.54583333333</v>
       </c>
       <c r="D48" s="1">
-        <v>44860</v>
+        <v>44861</v>
       </c>
       <c r="E48">
         <v>0.56999999999999995</v>
@@ -2963,7 +2963,7 @@
         <v>44853.447916666664</v>
       </c>
       <c r="D49" s="1">
-        <v>44860</v>
+        <v>44861</v>
       </c>
       <c r="E49">
         <v>0.69</v>
@@ -2998,7 +2998,7 @@
         <v>44853.55972222222</v>
       </c>
       <c r="D50" s="1">
-        <v>44860</v>
+        <v>44861</v>
       </c>
       <c r="E50">
         <v>0.63</v>
@@ -3033,7 +3033,7 @@
         <v>44853.465277777781</v>
       </c>
       <c r="D51" s="1">
-        <v>44860</v>
+        <v>44861</v>
       </c>
       <c r="E51">
         <v>0.54</v>
@@ -3068,7 +3068,7 @@
         <v>44853.488194444442</v>
       </c>
       <c r="D52" s="1">
-        <v>44860</v>
+        <v>44861</v>
       </c>
       <c r="E52">
         <v>0.39</v>
@@ -3103,7 +3103,7 @@
         <v>44853.598611111112</v>
       </c>
       <c r="D53" s="1">
-        <v>44860</v>
+        <v>44861</v>
       </c>
       <c r="E53">
         <v>0.27</v>
@@ -3138,7 +3138,7 @@
         <v>44853.538194444445</v>
       </c>
       <c r="D54" s="1">
-        <v>44860</v>
+        <v>44861</v>
       </c>
       <c r="E54">
         <v>0.6</v>
@@ -3173,7 +3173,7 @@
         <v>44853.638194444444</v>
       </c>
       <c r="D55" s="1">
-        <v>44860</v>
+        <v>44861</v>
       </c>
       <c r="E55">
         <v>0.75</v>
@@ -3208,7 +3208,7 @@
         <v>44853.385416666664</v>
       </c>
       <c r="D56" s="1">
-        <v>44860</v>
+        <v>44861</v>
       </c>
       <c r="E56">
         <v>0.67</v>
@@ -3243,7 +3243,7 @@
         <v>44853.385416666664</v>
       </c>
       <c r="D57" s="1">
-        <v>44860</v>
+        <v>44861</v>
       </c>
       <c r="E57">
         <v>0.71</v>
@@ -3278,7 +3278,7 @@
         <v>44853.692361111112</v>
       </c>
       <c r="D58" s="1">
-        <v>44860</v>
+        <v>44861</v>
       </c>
       <c r="E58">
         <v>0.81</v>
@@ -4223,7 +4223,7 @@
         <v>44979.552083333336</v>
       </c>
       <c r="D85" s="1">
-        <v>44980</v>
+        <v>44985</v>
       </c>
       <c r="E85">
         <v>0.54</v>
@@ -4258,7 +4258,7 @@
         <v>44979.552083333336</v>
       </c>
       <c r="D86" s="1">
-        <v>44980</v>
+        <v>44985</v>
       </c>
       <c r="E86">
         <v>0.59</v>
@@ -4293,7 +4293,7 @@
         <v>44979.496527777781</v>
       </c>
       <c r="D87" s="1">
-        <v>44980</v>
+        <v>44985</v>
       </c>
       <c r="E87">
         <v>0.81</v>
@@ -4328,7 +4328,7 @@
         <v>44979.427083333336</v>
       </c>
       <c r="D88" s="1">
-        <v>44980</v>
+        <v>44985</v>
       </c>
       <c r="E88">
         <v>0.51</v>
@@ -4363,7 +4363,7 @@
         <v>44979.520833333336</v>
       </c>
       <c r="D89" s="1">
-        <v>44980</v>
+        <v>44985</v>
       </c>
       <c r="E89">
         <v>0.79</v>
@@ -4398,7 +4398,7 @@
         <v>44979.438194444447</v>
       </c>
       <c r="D90" s="1">
-        <v>44980</v>
+        <v>44985</v>
       </c>
       <c r="E90">
         <v>0.74</v>
@@ -4433,7 +4433,7 @@
         <v>44979.447916666664</v>
       </c>
       <c r="D91" s="1">
-        <v>44980</v>
+        <v>44985</v>
       </c>
       <c r="E91">
         <v>0.6</v>
@@ -4468,7 +4468,7 @@
         <v>44979.413194444445</v>
       </c>
       <c r="D92" s="1">
-        <v>44980</v>
+        <v>44985</v>
       </c>
       <c r="E92">
         <v>0.28000000000000003</v>
@@ -4503,7 +4503,7 @@
         <v>44979.458333333336</v>
       </c>
       <c r="D93" s="1">
-        <v>44980</v>
+        <v>44985</v>
       </c>
       <c r="E93">
         <v>0.73</v>
@@ -4538,7 +4538,7 @@
         <v>44979.590277777781</v>
       </c>
       <c r="D94" s="1">
-        <v>44980</v>
+        <v>44985</v>
       </c>
       <c r="E94">
         <v>0.65</v>
@@ -4573,7 +4573,7 @@
         <v>44979.395833333336</v>
       </c>
       <c r="D95" s="1">
-        <v>44980</v>
+        <v>44985</v>
       </c>
       <c r="E95">
         <v>0.74</v>
@@ -4608,7 +4608,7 @@
         <v>44979.395833333336</v>
       </c>
       <c r="D96" s="1">
-        <v>44980</v>
+        <v>44985</v>
       </c>
       <c r="E96">
         <v>0.57999999999999996</v>
@@ -4643,7 +4643,7 @@
         <v>44984.5</v>
       </c>
       <c r="D97" s="1">
-        <v>44980</v>
+        <v>44985</v>
       </c>
       <c r="E97">
         <v>0.59</v>
@@ -4672,7 +4672,7 @@
         <v>44979.638888888891</v>
       </c>
       <c r="D98" s="1">
-        <v>44980</v>
+        <v>44985</v>
       </c>
       <c r="E98">
         <v>0.6</v>

</xml_diff>

<commit_message>
revised pipe grouping notebook; updated GA notebook with new pipe grouping options
</commit_message>
<xml_diff>
--- a/data/timeseries/raw/metrinet-calibration-records.xlsx
+++ b/data/timeseries/raw/metrinet-calibration-records.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\bradw\workspace\bayesian-wq-calibration\data\timeseries\raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62DB7565-998B-48DB-BAC0-83CA1880CD50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D18062A1-CF6F-45FF-B6FF-8E3DEC30E637}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2835" yWindow="5475" windowWidth="21600" windowHeight="12690" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="metrinet_calibration_records" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="720" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="721" uniqueCount="125">
   <si>
     <t>good_calib_event</t>
   </si>
@@ -650,18 +650,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K280"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B259" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F273" sqref="F273"/>
+    <sheetView tabSelected="1" topLeftCell="A248" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F277" sqref="F277"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="12.85546875" customWidth="1"/>
-    <col min="3" max="3" width="16.85546875" customWidth="1"/>
-    <col min="4" max="4" width="15.5703125" customWidth="1"/>
+    <col min="1" max="1" width="12.86328125" customWidth="1"/>
+    <col min="3" max="3" width="16.86328125" customWidth="1"/>
+    <col min="4" max="4" width="15.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -696,7 +696,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>1</v>
       </c>
@@ -731,7 +731,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>1</v>
       </c>
@@ -766,7 +766,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A4">
         <v>1</v>
       </c>
@@ -801,7 +801,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A5">
         <v>1</v>
       </c>
@@ -836,7 +836,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A6">
         <v>1</v>
       </c>
@@ -871,7 +871,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A7">
         <v>1</v>
       </c>
@@ -906,7 +906,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A8">
         <v>1</v>
       </c>
@@ -941,7 +941,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A9">
         <v>1</v>
       </c>
@@ -976,7 +976,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A10">
         <v>1</v>
       </c>
@@ -1011,7 +1011,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A11">
         <v>1</v>
       </c>
@@ -1046,7 +1046,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A12">
         <v>1</v>
       </c>
@@ -1081,7 +1081,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A13">
         <v>2</v>
       </c>
@@ -1116,7 +1116,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A14">
         <v>2</v>
       </c>
@@ -1151,7 +1151,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A15">
         <v>2</v>
       </c>
@@ -1186,7 +1186,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A16">
         <v>2</v>
       </c>
@@ -1221,7 +1221,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A17">
         <v>2</v>
       </c>
@@ -1256,7 +1256,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A18">
         <v>2</v>
       </c>
@@ -1291,7 +1291,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A19">
         <v>2</v>
       </c>
@@ -1326,7 +1326,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A20">
         <v>2</v>
       </c>
@@ -1361,7 +1361,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A21">
         <v>2</v>
       </c>
@@ -1396,7 +1396,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A22">
         <v>2</v>
       </c>
@@ -1431,7 +1431,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A23">
         <v>2</v>
       </c>
@@ -1466,7 +1466,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A24">
         <v>3</v>
       </c>
@@ -1501,7 +1501,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A25">
         <v>3</v>
       </c>
@@ -1536,7 +1536,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A26">
         <v>3</v>
       </c>
@@ -1571,7 +1571,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A27">
         <v>3</v>
       </c>
@@ -1606,7 +1606,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A28">
         <v>3</v>
       </c>
@@ -1641,7 +1641,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A29">
         <v>3</v>
       </c>
@@ -1676,7 +1676,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A30">
         <v>3</v>
       </c>
@@ -1711,7 +1711,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A31">
         <v>3</v>
       </c>
@@ -1746,7 +1746,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A32">
         <v>3</v>
       </c>
@@ -1781,7 +1781,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A33">
         <v>3</v>
       </c>
@@ -1816,7 +1816,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A34">
         <v>3</v>
       </c>
@@ -1851,7 +1851,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A35">
         <v>4</v>
       </c>
@@ -1886,7 +1886,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A36">
         <v>4</v>
       </c>
@@ -1921,7 +1921,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A37">
         <v>4</v>
       </c>
@@ -1956,7 +1956,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A38">
         <v>4</v>
       </c>
@@ -1991,7 +1991,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A39">
         <v>4</v>
       </c>
@@ -2026,7 +2026,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A40">
         <v>4</v>
       </c>
@@ -2061,7 +2061,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A41">
         <v>4</v>
       </c>
@@ -2096,7 +2096,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A42">
         <v>4</v>
       </c>
@@ -2131,7 +2131,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A43">
         <v>4</v>
       </c>
@@ -2166,7 +2166,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A44">
         <v>4</v>
       </c>
@@ -2201,7 +2201,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A45">
         <v>4</v>
       </c>
@@ -2236,7 +2236,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A46">
         <v>5</v>
       </c>
@@ -2271,7 +2271,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A47">
         <v>5</v>
       </c>
@@ -2306,7 +2306,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A48">
         <v>5</v>
       </c>
@@ -2341,7 +2341,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A49">
         <v>5</v>
       </c>
@@ -2376,7 +2376,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A50">
         <v>5</v>
       </c>
@@ -2411,7 +2411,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A51">
         <v>5</v>
       </c>
@@ -2446,7 +2446,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A52">
         <v>5</v>
       </c>
@@ -2481,7 +2481,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A53">
         <v>5</v>
       </c>
@@ -2516,7 +2516,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A54">
         <v>5</v>
       </c>
@@ -2551,7 +2551,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A55">
         <v>5</v>
       </c>
@@ -2586,7 +2586,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A56">
         <v>5</v>
       </c>
@@ -2621,7 +2621,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A57">
         <v>5</v>
       </c>
@@ -2656,7 +2656,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A58">
         <v>5</v>
       </c>
@@ -2691,7 +2691,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A59">
         <v>6</v>
       </c>
@@ -2726,7 +2726,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A60">
         <v>6</v>
       </c>
@@ -2761,7 +2761,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A61">
         <v>6</v>
       </c>
@@ -2796,7 +2796,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A62">
         <v>6</v>
       </c>
@@ -2831,7 +2831,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A63">
         <v>6</v>
       </c>
@@ -2866,7 +2866,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A64">
         <v>6</v>
       </c>
@@ -2901,7 +2901,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A65">
         <v>6</v>
       </c>
@@ -2936,7 +2936,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A66">
         <v>6</v>
       </c>
@@ -2971,7 +2971,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A67">
         <v>6</v>
       </c>
@@ -3006,7 +3006,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A68">
         <v>6</v>
       </c>
@@ -3041,7 +3041,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A69">
         <v>6</v>
       </c>
@@ -3076,7 +3076,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A70">
         <v>6</v>
       </c>
@@ -3111,7 +3111,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A71">
         <v>6</v>
       </c>
@@ -3146,7 +3146,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A72">
         <v>7</v>
       </c>
@@ -3181,7 +3181,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A73">
         <v>7</v>
       </c>
@@ -3216,7 +3216,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A74">
         <v>7</v>
       </c>
@@ -3251,7 +3251,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A75">
         <v>7</v>
       </c>
@@ -3286,7 +3286,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A76">
         <v>7</v>
       </c>
@@ -3321,7 +3321,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A77">
         <v>7</v>
       </c>
@@ -3356,7 +3356,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A78">
         <v>7</v>
       </c>
@@ -3391,7 +3391,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A79">
         <v>7</v>
       </c>
@@ -3426,7 +3426,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A80">
         <v>7</v>
       </c>
@@ -3461,7 +3461,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A81">
         <v>7</v>
       </c>
@@ -3496,7 +3496,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A82">
         <v>7</v>
       </c>
@@ -3531,7 +3531,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A83">
         <v>7</v>
       </c>
@@ -3566,7 +3566,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A84">
         <v>7</v>
       </c>
@@ -3601,7 +3601,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A85">
         <v>8</v>
       </c>
@@ -3636,7 +3636,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A86">
         <v>8</v>
       </c>
@@ -3671,7 +3671,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A87">
         <v>8</v>
       </c>
@@ -3706,7 +3706,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A88">
         <v>8</v>
       </c>
@@ -3741,7 +3741,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A89">
         <v>8</v>
       </c>
@@ -3776,7 +3776,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A90">
         <v>8</v>
       </c>
@@ -3811,7 +3811,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A91">
         <v>8</v>
       </c>
@@ -3846,7 +3846,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A92">
         <v>8</v>
       </c>
@@ -3881,7 +3881,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A93">
         <v>8</v>
       </c>
@@ -3916,7 +3916,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A94">
         <v>8</v>
       </c>
@@ -3951,7 +3951,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A95">
         <v>8</v>
       </c>
@@ -3986,7 +3986,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A96">
         <v>8</v>
       </c>
@@ -4021,7 +4021,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A97">
         <v>8</v>
       </c>
@@ -4050,7 +4050,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A98">
         <v>8</v>
       </c>
@@ -4085,7 +4085,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A99">
         <v>9</v>
       </c>
@@ -4120,7 +4120,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A100">
         <v>9</v>
       </c>
@@ -4155,7 +4155,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A101">
         <v>9</v>
       </c>
@@ -4190,7 +4190,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A102">
         <v>9</v>
       </c>
@@ -4225,7 +4225,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A103">
         <v>9</v>
       </c>
@@ -4260,7 +4260,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="104" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A104">
         <v>9</v>
       </c>
@@ -4295,7 +4295,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="105" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A105">
         <v>9</v>
       </c>
@@ -4330,7 +4330,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="106" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A106">
         <v>9</v>
       </c>
@@ -4365,7 +4365,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="107" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A107">
         <v>9</v>
       </c>
@@ -4400,7 +4400,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="108" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A108">
         <v>9</v>
       </c>
@@ -4435,7 +4435,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="109" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A109">
         <v>9</v>
       </c>
@@ -4470,7 +4470,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="110" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A110">
         <v>9</v>
       </c>
@@ -4505,7 +4505,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="111" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A111">
         <v>9</v>
       </c>
@@ -4540,7 +4540,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="112" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A112">
         <v>10</v>
       </c>
@@ -4575,7 +4575,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="113" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A113">
         <v>10</v>
       </c>
@@ -4610,7 +4610,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="114" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A114">
         <v>10</v>
       </c>
@@ -4645,7 +4645,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="115" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A115">
         <v>10</v>
       </c>
@@ -4680,7 +4680,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="116" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A116">
         <v>10</v>
       </c>
@@ -4715,7 +4715,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="117" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A117">
         <v>10</v>
       </c>
@@ -4747,7 +4747,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="118" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A118">
         <v>10</v>
       </c>
@@ -4782,7 +4782,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="119" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A119">
         <v>10</v>
       </c>
@@ -4817,7 +4817,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="120" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A120">
         <v>10</v>
       </c>
@@ -4852,7 +4852,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="121" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A121">
         <v>10</v>
       </c>
@@ -4887,7 +4887,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="122" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A122">
         <v>10</v>
       </c>
@@ -4922,7 +4922,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="123" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A123">
         <v>10</v>
       </c>
@@ -4957,7 +4957,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="124" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A124">
         <v>10</v>
       </c>
@@ -4992,7 +4992,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="125" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A125">
         <v>10</v>
       </c>
@@ -5027,7 +5027,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="126" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A126">
         <v>10</v>
       </c>
@@ -5062,7 +5062,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="127" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A127">
         <v>11</v>
       </c>
@@ -5097,7 +5097,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="128" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A128">
         <v>11</v>
       </c>
@@ -5132,7 +5132,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="129" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A129">
         <v>11</v>
       </c>
@@ -5167,7 +5167,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="130" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A130">
         <v>11</v>
       </c>
@@ -5202,7 +5202,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="131" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A131">
         <v>11</v>
       </c>
@@ -5237,7 +5237,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="132" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A132">
         <v>11</v>
       </c>
@@ -5272,7 +5272,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="133" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A133">
         <v>11</v>
       </c>
@@ -5307,7 +5307,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="134" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A134">
         <v>11</v>
       </c>
@@ -5342,7 +5342,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="135" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A135">
         <v>11</v>
       </c>
@@ -5377,7 +5377,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="136" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A136">
         <v>11</v>
       </c>
@@ -5412,7 +5412,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="137" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A137">
         <v>11</v>
       </c>
@@ -5447,7 +5447,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="138" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A138">
         <v>11</v>
       </c>
@@ -5482,7 +5482,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="139" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A139">
         <v>11</v>
       </c>
@@ -5517,7 +5517,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="140" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A140">
         <v>12</v>
       </c>
@@ -5552,7 +5552,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="141" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A141">
         <v>12</v>
       </c>
@@ -5587,7 +5587,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="142" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A142">
         <v>12</v>
       </c>
@@ -5622,7 +5622,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="143" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A143">
         <v>12</v>
       </c>
@@ -5657,7 +5657,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="144" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A144">
         <v>12</v>
       </c>
@@ -5692,7 +5692,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="145" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A145">
         <v>12</v>
       </c>
@@ -5727,7 +5727,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="146" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A146">
         <v>12</v>
       </c>
@@ -5762,7 +5762,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="147" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A147">
         <v>12</v>
       </c>
@@ -5797,7 +5797,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="148" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A148">
         <v>12</v>
       </c>
@@ -5832,7 +5832,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="149" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A149">
         <v>12</v>
       </c>
@@ -5867,7 +5867,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="150" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A150">
         <v>12</v>
       </c>
@@ -5902,7 +5902,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="151" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A151">
         <v>12</v>
       </c>
@@ -5937,7 +5937,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="152" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A152">
         <v>12</v>
       </c>
@@ -5972,7 +5972,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="153" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A153">
         <v>12</v>
       </c>
@@ -6007,7 +6007,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="154" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A154">
         <v>12</v>
       </c>
@@ -6042,7 +6042,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="155" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A155">
         <v>13</v>
       </c>
@@ -6074,7 +6074,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="156" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A156">
         <v>13</v>
       </c>
@@ -6106,7 +6106,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="157" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A157">
         <v>13</v>
       </c>
@@ -6138,7 +6138,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="158" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A158">
         <v>13</v>
       </c>
@@ -6170,7 +6170,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="159" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A159">
         <v>13</v>
       </c>
@@ -6202,7 +6202,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="160" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A160">
         <v>13</v>
       </c>
@@ -6234,7 +6234,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="161" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A161">
         <v>13</v>
       </c>
@@ -6266,7 +6266,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="162" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A162">
         <v>13</v>
       </c>
@@ -6298,7 +6298,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="163" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A163">
         <v>13</v>
       </c>
@@ -6330,7 +6330,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="164" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A164">
         <v>13</v>
       </c>
@@ -6362,7 +6362,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="165" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A165">
         <v>13</v>
       </c>
@@ -6394,7 +6394,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="166" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A166">
         <v>13</v>
       </c>
@@ -6426,7 +6426,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="167" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A167">
         <v>13</v>
       </c>
@@ -6458,7 +6458,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="168" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A168">
         <v>13</v>
       </c>
@@ -6490,7 +6490,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="169" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A169">
         <v>14</v>
       </c>
@@ -6522,7 +6522,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="170" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A170">
         <v>14</v>
       </c>
@@ -6554,7 +6554,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="171" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A171">
         <v>14</v>
       </c>
@@ -6586,7 +6586,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="172" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A172">
         <v>14</v>
       </c>
@@ -6618,7 +6618,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="173" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A173">
         <v>14</v>
       </c>
@@ -6650,7 +6650,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="174" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A174">
         <v>14</v>
       </c>
@@ -6682,7 +6682,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="175" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A175">
         <v>14</v>
       </c>
@@ -6714,7 +6714,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="176" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A176">
         <v>14</v>
       </c>
@@ -6746,7 +6746,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="177" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A177">
         <v>14</v>
       </c>
@@ -6778,7 +6778,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="178" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A178">
         <v>14</v>
       </c>
@@ -6810,7 +6810,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="179" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A179">
         <v>14</v>
       </c>
@@ -6842,7 +6842,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="180" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A180">
         <v>14</v>
       </c>
@@ -6874,7 +6874,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="181" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A181">
         <v>14</v>
       </c>
@@ -6906,7 +6906,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="182" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A182">
         <v>14</v>
       </c>
@@ -6938,7 +6938,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="183" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A183">
         <v>15</v>
       </c>
@@ -6970,7 +6970,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="184" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A184">
         <v>15</v>
       </c>
@@ -7002,7 +7002,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="185" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A185">
         <v>15</v>
       </c>
@@ -7034,7 +7034,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="186" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A186">
         <v>15</v>
       </c>
@@ -7066,7 +7066,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="187" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A187">
         <v>15</v>
       </c>
@@ -7098,7 +7098,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="188" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A188">
         <v>15</v>
       </c>
@@ -7130,7 +7130,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="189" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A189">
         <v>15</v>
       </c>
@@ -7162,7 +7162,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="190" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A190">
         <v>15</v>
       </c>
@@ -7191,7 +7191,7 @@
         <v>0.56999999999999995</v>
       </c>
     </row>
-    <row r="191" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A191">
         <v>15</v>
       </c>
@@ -7223,7 +7223,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="192" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A192">
         <v>15</v>
       </c>
@@ -7255,7 +7255,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="193" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A193">
         <v>15</v>
       </c>
@@ -7287,7 +7287,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="194" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A194">
         <v>15</v>
       </c>
@@ -7319,7 +7319,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="195" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A195">
         <v>15</v>
       </c>
@@ -7351,7 +7351,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="196" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A196">
         <v>15</v>
       </c>
@@ -7383,7 +7383,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="197" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A197">
         <v>16</v>
       </c>
@@ -7415,7 +7415,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="198" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A198">
         <v>16</v>
       </c>
@@ -7447,7 +7447,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="199" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A199">
         <v>16</v>
       </c>
@@ -7479,7 +7479,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="200" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A200">
         <v>16</v>
       </c>
@@ -7511,7 +7511,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="201" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A201">
         <v>16</v>
       </c>
@@ -7543,7 +7543,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="202" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A202">
         <v>16</v>
       </c>
@@ -7575,7 +7575,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="203" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A203">
         <v>16</v>
       </c>
@@ -7607,7 +7607,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="204" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A204">
         <v>16</v>
       </c>
@@ -7639,7 +7639,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="205" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A205">
         <v>16</v>
       </c>
@@ -7671,7 +7671,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="206" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A206">
         <v>16</v>
       </c>
@@ -7703,7 +7703,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="207" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A207">
         <v>16</v>
       </c>
@@ -7735,7 +7735,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="208" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A208">
         <v>16</v>
       </c>
@@ -7767,7 +7767,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="209" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A209">
         <v>16</v>
       </c>
@@ -7799,7 +7799,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="210" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A210">
         <v>16</v>
       </c>
@@ -7831,7 +7831,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="211" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A211">
         <v>17</v>
       </c>
@@ -7863,7 +7863,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="212" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A212">
         <v>17</v>
       </c>
@@ -7895,7 +7895,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="213" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A213">
         <v>17</v>
       </c>
@@ -7927,7 +7927,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="214" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A214">
         <v>17</v>
       </c>
@@ -7956,7 +7956,7 @@
         <v>1.84</v>
       </c>
     </row>
-    <row r="215" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A215">
         <v>17</v>
       </c>
@@ -7988,7 +7988,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="216" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A216">
         <v>17</v>
       </c>
@@ -8020,7 +8020,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="217" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A217">
         <v>17</v>
       </c>
@@ -8049,7 +8049,7 @@
         <v>0.53</v>
       </c>
     </row>
-    <row r="218" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A218">
         <v>17</v>
       </c>
@@ -8081,7 +8081,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="219" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A219">
         <v>17</v>
       </c>
@@ -8113,7 +8113,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="220" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A220">
         <v>17</v>
       </c>
@@ -8145,7 +8145,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="221" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A221">
         <v>17</v>
       </c>
@@ -8177,7 +8177,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="222" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A222">
         <v>17</v>
       </c>
@@ -8209,7 +8209,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="223" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A223">
         <v>17</v>
       </c>
@@ -8241,7 +8241,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="224" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A224">
         <v>17</v>
       </c>
@@ -8273,7 +8273,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="225" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A225">
         <v>18</v>
       </c>
@@ -8305,7 +8305,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="226" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A226">
         <v>18</v>
       </c>
@@ -8337,7 +8337,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="227" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A227">
         <v>18</v>
       </c>
@@ -8369,7 +8369,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="228" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A228">
         <v>18</v>
       </c>
@@ -8401,7 +8401,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="229" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A229">
         <v>18</v>
       </c>
@@ -8433,7 +8433,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="230" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A230">
         <v>18</v>
       </c>
@@ -8465,7 +8465,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="231" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A231">
         <v>18</v>
       </c>
@@ -8497,7 +8497,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="232" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A232">
         <v>18</v>
       </c>
@@ -8529,7 +8529,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="233" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A233">
         <v>18</v>
       </c>
@@ -8558,7 +8558,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="234" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A234">
         <v>18</v>
       </c>
@@ -8590,7 +8590,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="235" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A235">
         <v>18</v>
       </c>
@@ -8622,7 +8622,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="236" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A236">
         <v>18</v>
       </c>
@@ -8654,7 +8654,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="237" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A237">
         <v>18</v>
       </c>
@@ -8686,7 +8686,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="238" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A238">
         <v>18</v>
       </c>
@@ -8718,7 +8718,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="239" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A239">
         <v>19</v>
       </c>
@@ -8750,7 +8750,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="240" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A240">
         <v>19</v>
       </c>
@@ -8782,7 +8782,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="241" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A241">
         <v>19</v>
       </c>
@@ -8814,7 +8814,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="242" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A242">
         <v>19</v>
       </c>
@@ -8846,7 +8846,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="243" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A243">
         <v>19</v>
       </c>
@@ -8878,7 +8878,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="244" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A244">
         <v>19</v>
       </c>
@@ -8910,7 +8910,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="245" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A245">
         <v>19</v>
       </c>
@@ -8942,7 +8942,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="246" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A246">
         <v>19</v>
       </c>
@@ -8974,7 +8974,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="247" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A247">
         <v>19</v>
       </c>
@@ -9006,7 +9006,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="248" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A248">
         <v>19</v>
       </c>
@@ -9038,7 +9038,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="249" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A249">
         <v>19</v>
       </c>
@@ -9070,7 +9070,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="250" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A250">
         <v>19</v>
       </c>
@@ -9102,7 +9102,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="251" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A251">
         <v>19</v>
       </c>
@@ -9134,7 +9134,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="252" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A252">
         <v>19</v>
       </c>
@@ -9166,7 +9166,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="253" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A253">
         <v>20</v>
       </c>
@@ -9187,7 +9187,7 @@
         <v>0.48333333333333334</v>
       </c>
       <c r="G253">
-        <f t="shared" ref="G253:G266" si="0">E253-F253</f>
+        <f t="shared" ref="G253:G270" si="0">E253-F253</f>
         <v>6.6666666666666541E-3</v>
       </c>
       <c r="H253" t="s">
@@ -9200,7 +9200,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="254" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A254">
         <v>20</v>
       </c>
@@ -9234,7 +9234,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="255" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A255">
         <v>20</v>
       </c>
@@ -9268,7 +9268,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="256" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A256">
         <v>20</v>
       </c>
@@ -9302,7 +9302,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="257" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A257">
         <v>20</v>
       </c>
@@ -9336,7 +9336,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="258" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A258">
         <v>20</v>
       </c>
@@ -9370,7 +9370,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="259" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A259">
         <v>20</v>
       </c>
@@ -9404,7 +9404,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="260" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A260">
         <v>20</v>
       </c>
@@ -9437,7 +9437,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="261" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A261">
         <v>20</v>
       </c>
@@ -9471,7 +9471,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="262" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A262">
         <v>20</v>
       </c>
@@ -9505,7 +9505,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="263" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A263">
         <v>20</v>
       </c>
@@ -9539,7 +9539,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="264" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A264">
         <v>20</v>
       </c>
@@ -9573,7 +9573,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="265" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A265">
         <v>20</v>
       </c>
@@ -9607,7 +9607,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="266" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A266">
         <v>20</v>
       </c>
@@ -9641,7 +9641,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="267" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A267">
         <v>21</v>
       </c>
@@ -9649,24 +9649,24 @@
         <v>11</v>
       </c>
       <c r="C267" s="1">
-        <v>45616.732638888891</v>
+        <v>45642.645833333336</v>
       </c>
       <c r="D267" s="1">
-        <v>45621</v>
+        <v>45643</v>
       </c>
       <c r="E267">
-        <v>1.1000000000000001</v>
+        <v>0.54</v>
       </c>
       <c r="F267">
-        <f>AVERAGE(0.91, 0.93, 0.93)</f>
-        <v>0.92333333333333334</v>
+        <f>AVERAGE(0.55, 0.53, 0.56)</f>
+        <v>0.54666666666666675</v>
       </c>
       <c r="G267">
-        <f t="shared" ref="G267:G280" si="1">E267-F267</f>
-        <v>0.17666666666666675</v>
+        <f t="shared" si="0"/>
+        <v>-6.6666666666667096E-3</v>
       </c>
       <c r="H267" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="I267">
         <v>2.11</v>
@@ -9675,7 +9675,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="268" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A268">
         <v>21</v>
       </c>
@@ -9683,24 +9683,24 @@
         <v>59</v>
       </c>
       <c r="C268" s="1">
-        <v>45616.732638888891</v>
+        <v>45642.645833333336</v>
       </c>
       <c r="D268" s="1">
-        <v>45621</v>
+        <v>45643</v>
       </c>
       <c r="E268">
-        <v>1.1499999999999999</v>
+        <v>0.53</v>
       </c>
       <c r="F268">
-        <f>AVERAGE(0.91, 0.93, 0.93)</f>
-        <v>0.92333333333333334</v>
+        <f>AVERAGE(0.55, 0.53, 0.56)</f>
+        <v>0.54666666666666675</v>
       </c>
       <c r="G268">
-        <f t="shared" si="1"/>
-        <v>0.22666666666666657</v>
+        <f t="shared" si="0"/>
+        <v>-1.6666666666666718E-2</v>
       </c>
       <c r="H268" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="I268">
         <v>2.06</v>
@@ -9709,7 +9709,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="269" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A269">
         <v>21</v>
       </c>
@@ -9717,21 +9717,21 @@
         <v>14</v>
       </c>
       <c r="C269" s="1">
-        <v>45616.663194444445</v>
+        <v>45642.645833333336</v>
       </c>
       <c r="D269" s="1">
-        <v>45621</v>
+        <v>45643</v>
       </c>
       <c r="E269">
-        <v>0.88</v>
+        <v>0.5</v>
       </c>
       <c r="F269">
-        <f>AVERAGE(0.89,0.88,0.88)</f>
-        <v>0.8833333333333333</v>
+        <f>AVERAGE(0.51, 0.51, 0.52)</f>
+        <v>0.51333333333333331</v>
       </c>
       <c r="G269">
-        <f t="shared" si="1"/>
-        <v>-3.3333333333332993E-3</v>
+        <f t="shared" si="0"/>
+        <v>-1.3333333333333308E-2</v>
       </c>
       <c r="H269" t="s">
         <v>12</v>
@@ -9740,10 +9740,10 @@
         <v>1.98</v>
       </c>
       <c r="J269">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="270" spans="1:10" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="270" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A270">
         <v>21</v>
       </c>
@@ -9751,27 +9751,33 @@
         <v>17</v>
       </c>
       <c r="C270" s="1">
-        <v>45616.515277777777</v>
+        <v>45642.426388888889</v>
       </c>
       <c r="D270" s="1">
-        <v>45621</v>
+        <v>45643</v>
+      </c>
+      <c r="E270">
+        <v>0.53</v>
       </c>
       <c r="F270">
-        <f>AVERAGE(0.83,0.84,0.87,0.88)</f>
-        <v>0.85499999999999998</v>
+        <f>AVERAGE(0.55, 0.55, 0.53)</f>
+        <v>0.54333333333333333</v>
       </c>
       <c r="G270">
-        <f t="shared" si="1"/>
-        <v>-0.85499999999999998</v>
+        <f t="shared" si="0"/>
+        <v>-1.3333333333333308E-2</v>
+      </c>
+      <c r="H270" t="s">
+        <v>12</v>
       </c>
       <c r="I270">
         <v>1.62</v>
       </c>
       <c r="J270">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="271" spans="1:10" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="271" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A271">
         <v>21</v>
       </c>
@@ -9779,33 +9785,33 @@
         <v>19</v>
       </c>
       <c r="C271" s="1">
-        <v>45616.682638888888</v>
+        <v>45642.618055555555</v>
       </c>
       <c r="D271" s="1">
-        <v>45621</v>
+        <v>45643</v>
       </c>
       <c r="E271">
-        <v>0.85</v>
+        <v>0.49</v>
       </c>
       <c r="F271">
-        <f>AVERAGE(0.74,0.71,0.71)</f>
-        <v>0.72000000000000008</v>
+        <f>AVERAGE(0.5, 0.51, 0.52)</f>
+        <v>0.51</v>
       </c>
       <c r="G271">
-        <f t="shared" si="1"/>
-        <v>0.12999999999999989</v>
+        <f t="shared" ref="G271:G273" si="1">E271-F271</f>
+        <v>-2.0000000000000018E-2</v>
       </c>
       <c r="H271" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="I271">
-        <v>2.15</v>
+        <v>2.5</v>
       </c>
       <c r="J271">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="272" spans="1:10" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="272" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A272">
         <v>21</v>
       </c>
@@ -9813,33 +9819,33 @@
         <v>119</v>
       </c>
       <c r="C272" s="1">
-        <v>45616.684027777781</v>
+        <v>45642.618055555555</v>
       </c>
       <c r="D272" s="1">
-        <v>45621</v>
+        <v>45643</v>
       </c>
       <c r="E272">
-        <v>0.85</v>
+        <v>0.5</v>
       </c>
       <c r="F272">
-        <f>AVERAGE(0.74,0.71,0.71)</f>
-        <v>0.72000000000000008</v>
+        <f>AVERAGE(0.5, 0.51, 0.52)</f>
+        <v>0.51</v>
       </c>
       <c r="G272">
         <f t="shared" si="1"/>
-        <v>0.12999999999999989</v>
+        <v>-1.0000000000000009E-2</v>
       </c>
       <c r="H272" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="I272">
         <v>2.17</v>
       </c>
       <c r="J272">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="273" spans="1:10" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="273" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A273">
         <v>21</v>
       </c>
@@ -9847,24 +9853,24 @@
         <v>21</v>
       </c>
       <c r="C273" s="1">
-        <v>45616.530555555553</v>
+        <v>45642.439583333333</v>
       </c>
       <c r="D273" s="1">
-        <v>45621</v>
+        <v>45643</v>
       </c>
       <c r="E273">
-        <v>1.1299999999999999</v>
+        <v>0.54</v>
       </c>
       <c r="F273">
-        <f>AVERAGE(0.87,0.87,0.87)</f>
-        <v>0.87</v>
+        <f>AVERAGE(0.56, 0.57, 0.57)</f>
+        <v>0.56666666666666654</v>
       </c>
       <c r="G273">
         <f t="shared" si="1"/>
-        <v>0.2599999999999999</v>
+        <v>-2.6666666666666505E-2</v>
       </c>
       <c r="H273" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="I273">
         <v>0.69</v>
@@ -9873,7 +9879,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="274" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A274">
         <v>21</v>
       </c>
@@ -9881,21 +9887,21 @@
         <v>23</v>
       </c>
       <c r="C274" s="1">
-        <v>45616.625</v>
+        <v>45642.466666666667</v>
       </c>
       <c r="D274" s="1">
-        <v>45621</v>
+        <v>45643</v>
       </c>
       <c r="E274">
-        <v>0.71</v>
+        <v>0.47</v>
       </c>
       <c r="F274">
-        <f>AVERAGE(0.72,0.72,0.73)</f>
-        <v>0.72333333333333327</v>
+        <f>AVERAGE(0.45, 0.51, 0.45)</f>
+        <v>0.47</v>
       </c>
       <c r="G274">
-        <f t="shared" si="1"/>
-        <v>-1.3333333333333308E-2</v>
+        <f t="shared" ref="G274" si="2">E274-F274</f>
+        <v>0</v>
       </c>
       <c r="H274" t="s">
         <v>12</v>
@@ -9904,10 +9910,10 @@
         <v>2.08</v>
       </c>
       <c r="J274">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="275" spans="1:10" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="275" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A275">
         <v>21</v>
       </c>
@@ -9915,24 +9921,24 @@
         <v>25</v>
       </c>
       <c r="C275" s="1">
-        <v>45616.491666666669</v>
+        <v>45642.401388888888</v>
       </c>
       <c r="D275" s="1">
-        <v>45621</v>
+        <v>45643</v>
       </c>
       <c r="E275">
-        <v>0.83</v>
+        <v>0.4</v>
       </c>
       <c r="F275">
-        <f>AVERAGE(0.53,0.5,0.53,0.54)</f>
-        <v>0.52500000000000002</v>
+        <f>AVERAGE(0.38, 0.39, 0.43)</f>
+        <v>0.39999999999999997</v>
       </c>
       <c r="G275">
-        <f t="shared" si="1"/>
-        <v>0.30499999999999994</v>
+        <f t="shared" ref="G275:G280" si="3">E275-F275</f>
+        <v>0</v>
       </c>
       <c r="H275" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="I275">
         <v>1.65</v>
@@ -9941,7 +9947,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="276" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A276">
         <v>21</v>
       </c>
@@ -9949,21 +9955,21 @@
         <v>26</v>
       </c>
       <c r="C276" s="1">
-        <v>45616.640277777777</v>
+        <v>45642.517361111109</v>
       </c>
       <c r="D276" s="1">
-        <v>45621</v>
+        <v>45643</v>
       </c>
       <c r="E276">
-        <v>0.86</v>
+        <v>0.52</v>
       </c>
       <c r="F276">
-        <f>AVERAGE(0.87,0.82,0.85)</f>
-        <v>0.84666666666666668</v>
+        <f>AVERAGE(0.5, 0.49, 0.49)</f>
+        <v>0.49333333333333335</v>
       </c>
       <c r="G276">
-        <f t="shared" si="1"/>
-        <v>1.3333333333333308E-2</v>
+        <f t="shared" si="3"/>
+        <v>2.6666666666666672E-2</v>
       </c>
       <c r="H276" t="s">
         <v>12</v>
@@ -9972,10 +9978,10 @@
         <v>1.89</v>
       </c>
       <c r="J276">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="277" spans="1:10" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="277" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A277">
         <v>21</v>
       </c>
@@ -9983,33 +9989,33 @@
         <v>122</v>
       </c>
       <c r="C277" s="1">
-        <v>45616.638888888891</v>
+        <v>45642.517361111109</v>
       </c>
       <c r="D277" s="1">
-        <v>45621</v>
+        <v>45643</v>
       </c>
       <c r="E277">
-        <v>0.91</v>
+        <v>0.51</v>
       </c>
       <c r="F277">
-        <f>AVERAGE(0.87,0.82,0.85)</f>
-        <v>0.84666666666666668</v>
+        <f>AVERAGE(0.5, 0.49, 0.49)</f>
+        <v>0.49333333333333335</v>
       </c>
       <c r="G277">
-        <f t="shared" si="1"/>
-        <v>6.3333333333333353E-2</v>
+        <f t="shared" si="3"/>
+        <v>1.6666666666666663E-2</v>
       </c>
       <c r="H277" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="I277">
         <v>1.9</v>
       </c>
       <c r="J277">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="278" spans="1:10" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="278" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A278">
         <v>21</v>
       </c>
@@ -10017,33 +10023,33 @@
         <v>27</v>
       </c>
       <c r="C278" s="1">
-        <v>45616.755555555559</v>
+        <v>45642.663194444445</v>
       </c>
       <c r="D278" s="1">
-        <v>45621</v>
+        <v>45643</v>
       </c>
       <c r="E278">
-        <v>1.01</v>
+        <v>0.63</v>
       </c>
       <c r="F278">
-        <f>AVERAGE(0.96,1.01,0.94)</f>
-        <v>0.97000000000000008</v>
+        <f>AVERAGE(0.64, 0.65, 0.63)</f>
+        <v>0.64</v>
       </c>
       <c r="G278">
-        <f t="shared" si="1"/>
-        <v>3.9999999999999925E-2</v>
+        <f t="shared" si="3"/>
+        <v>-1.0000000000000009E-2</v>
       </c>
       <c r="H278" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="I278">
         <v>1.96</v>
       </c>
       <c r="J278">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="279" spans="1:10" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="279" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A279">
         <v>21</v>
       </c>
@@ -10051,33 +10057,33 @@
         <v>29</v>
       </c>
       <c r="C279" s="1">
-        <v>45616.402777777781</v>
+        <v>45642.380555555559</v>
       </c>
       <c r="D279" s="1">
-        <v>45621</v>
+        <v>45643</v>
       </c>
       <c r="E279">
-        <v>1</v>
+        <v>0.6</v>
       </c>
       <c r="F279">
-        <f>AVERAGE(0.9,0.93,0.91)</f>
-        <v>0.91333333333333344</v>
+        <f>AVERAGE(0.66, 0.66, 0.65)</f>
+        <v>0.65666666666666673</v>
       </c>
       <c r="G279">
-        <f t="shared" si="1"/>
-        <v>8.6666666666666559E-2</v>
+        <f t="shared" si="3"/>
+        <v>-5.6666666666666754E-2</v>
       </c>
       <c r="H279" t="s">
         <v>15</v>
       </c>
       <c r="I279">
-        <v>1.96</v>
+        <v>1.77</v>
       </c>
       <c r="J279">
         <v>10</v>
       </c>
     </row>
-    <row r="280" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A280">
         <v>21</v>
       </c>
@@ -10085,27 +10091,27 @@
         <v>67</v>
       </c>
       <c r="C280" s="1">
-        <v>45616.402777777781</v>
+        <v>45642.380555555559</v>
       </c>
       <c r="D280" s="1">
-        <v>45621</v>
+        <v>45643</v>
       </c>
       <c r="E280">
-        <v>1.03</v>
+        <v>0.59</v>
       </c>
       <c r="F280">
-        <f>AVERAGE(0.9,0.93,0.91)</f>
-        <v>0.91333333333333344</v>
+        <f>AVERAGE(0.66, 0.66, 0.65)</f>
+        <v>0.65666666666666673</v>
       </c>
       <c r="G280">
-        <f t="shared" si="1"/>
-        <v>0.11666666666666659</v>
+        <f t="shared" si="3"/>
+        <v>-6.6666666666666763E-2</v>
       </c>
       <c r="H280" t="s">
         <v>15</v>
       </c>
       <c r="I280">
-        <v>2.0099999999999998</v>
+        <v>1.81</v>
       </c>
       <c r="J280">
         <v>10</v>

</xml_diff>

<commit_message>
small updates to network plotting code
</commit_message>
<xml_diff>
--- a/data/timeseries/raw/metrinet-calibration-records.xlsx
+++ b/data/timeseries/raw/metrinet-calibration-records.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10112"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\bradw\workspace\bayesian-wq-calibration\data\timeseries\raw\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bradwjenks/Code/PhD/bayesian-wq-calibration/data/timeseries/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D18062A1-CF6F-45FF-B6FF-8E3DEC30E637}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE1200ED-FD1D-AA4B-B6A3-693F2F7C0BF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="29000" windowHeight="17460" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="metrinet_calibration_records" sheetId="1" r:id="rId1"/>
@@ -650,18 +650,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K280"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A248" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F277" sqref="F277"/>
+    <sheetView tabSelected="1" topLeftCell="A255" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M271" sqref="M271"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.86328125" customWidth="1"/>
-    <col min="3" max="3" width="16.86328125" customWidth="1"/>
-    <col min="4" max="4" width="15.59765625" customWidth="1"/>
+    <col min="1" max="1" width="12.83203125" customWidth="1"/>
+    <col min="3" max="3" width="16.83203125" customWidth="1"/>
+    <col min="4" max="4" width="15.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -696,7 +696,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -731,7 +731,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -766,7 +766,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1</v>
       </c>
@@ -801,7 +801,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1</v>
       </c>
@@ -836,7 +836,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>1</v>
       </c>
@@ -871,7 +871,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>1</v>
       </c>
@@ -906,7 +906,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>1</v>
       </c>
@@ -941,7 +941,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>1</v>
       </c>
@@ -976,7 +976,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>1</v>
       </c>
@@ -1011,7 +1011,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>1</v>
       </c>
@@ -1046,7 +1046,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>1</v>
       </c>
@@ -1081,7 +1081,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>2</v>
       </c>
@@ -1116,7 +1116,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>2</v>
       </c>
@@ -1151,7 +1151,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>2</v>
       </c>
@@ -1186,7 +1186,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>2</v>
       </c>
@@ -1221,7 +1221,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>2</v>
       </c>
@@ -1256,7 +1256,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>2</v>
       </c>
@@ -1291,7 +1291,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>2</v>
       </c>
@@ -1326,7 +1326,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>2</v>
       </c>
@@ -1361,7 +1361,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>2</v>
       </c>
@@ -1396,7 +1396,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>2</v>
       </c>
@@ -1431,7 +1431,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>2</v>
       </c>
@@ -1466,7 +1466,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>3</v>
       </c>
@@ -1501,7 +1501,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>3</v>
       </c>
@@ -1536,7 +1536,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>3</v>
       </c>
@@ -1571,7 +1571,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>3</v>
       </c>
@@ -1606,7 +1606,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>3</v>
       </c>
@@ -1641,7 +1641,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>3</v>
       </c>
@@ -1676,7 +1676,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>3</v>
       </c>
@@ -1711,7 +1711,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>3</v>
       </c>
@@ -1746,7 +1746,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>3</v>
       </c>
@@ -1781,7 +1781,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>3</v>
       </c>
@@ -1816,7 +1816,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>3</v>
       </c>
@@ -1851,7 +1851,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>4</v>
       </c>
@@ -1886,7 +1886,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>4</v>
       </c>
@@ -1921,7 +1921,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>4</v>
       </c>
@@ -1956,7 +1956,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>4</v>
       </c>
@@ -1991,7 +1991,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>4</v>
       </c>
@@ -2026,7 +2026,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>4</v>
       </c>
@@ -2061,7 +2061,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>4</v>
       </c>
@@ -2096,7 +2096,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>4</v>
       </c>
@@ -2131,7 +2131,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>4</v>
       </c>
@@ -2166,7 +2166,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>4</v>
       </c>
@@ -2201,7 +2201,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>4</v>
       </c>
@@ -2236,7 +2236,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>5</v>
       </c>
@@ -2271,7 +2271,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>5</v>
       </c>
@@ -2306,7 +2306,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>5</v>
       </c>
@@ -2341,7 +2341,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>5</v>
       </c>
@@ -2376,7 +2376,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>5</v>
       </c>
@@ -2411,7 +2411,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>5</v>
       </c>
@@ -2446,7 +2446,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>5</v>
       </c>
@@ -2481,7 +2481,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>5</v>
       </c>
@@ -2516,7 +2516,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>5</v>
       </c>
@@ -2551,7 +2551,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>5</v>
       </c>
@@ -2586,7 +2586,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>5</v>
       </c>
@@ -2621,7 +2621,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>5</v>
       </c>
@@ -2656,7 +2656,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>5</v>
       </c>
@@ -2691,7 +2691,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>6</v>
       </c>
@@ -2726,7 +2726,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>6</v>
       </c>
@@ -2761,7 +2761,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>6</v>
       </c>
@@ -2796,7 +2796,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>6</v>
       </c>
@@ -2831,7 +2831,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>6</v>
       </c>
@@ -2866,7 +2866,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>6</v>
       </c>
@@ -2901,7 +2901,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>6</v>
       </c>
@@ -2936,7 +2936,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>6</v>
       </c>
@@ -2971,7 +2971,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>6</v>
       </c>
@@ -3006,7 +3006,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>6</v>
       </c>
@@ -3041,7 +3041,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>6</v>
       </c>
@@ -3076,7 +3076,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>6</v>
       </c>
@@ -3111,7 +3111,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>6</v>
       </c>
@@ -3146,7 +3146,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A72">
         <v>7</v>
       </c>
@@ -3181,7 +3181,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A73">
         <v>7</v>
       </c>
@@ -3216,7 +3216,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A74">
         <v>7</v>
       </c>
@@ -3251,7 +3251,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A75">
         <v>7</v>
       </c>
@@ -3286,7 +3286,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A76">
         <v>7</v>
       </c>
@@ -3321,7 +3321,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A77">
         <v>7</v>
       </c>
@@ -3356,7 +3356,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A78">
         <v>7</v>
       </c>
@@ -3391,7 +3391,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A79">
         <v>7</v>
       </c>
@@ -3426,7 +3426,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A80">
         <v>7</v>
       </c>
@@ -3461,7 +3461,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A81">
         <v>7</v>
       </c>
@@ -3496,7 +3496,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A82">
         <v>7</v>
       </c>
@@ -3531,7 +3531,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A83">
         <v>7</v>
       </c>
@@ -3566,7 +3566,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A84">
         <v>7</v>
       </c>
@@ -3601,7 +3601,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A85">
         <v>8</v>
       </c>
@@ -3636,7 +3636,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A86">
         <v>8</v>
       </c>
@@ -3671,7 +3671,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A87">
         <v>8</v>
       </c>
@@ -3706,7 +3706,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A88">
         <v>8</v>
       </c>
@@ -3741,7 +3741,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A89">
         <v>8</v>
       </c>
@@ -3776,7 +3776,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A90">
         <v>8</v>
       </c>
@@ -3811,7 +3811,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A91">
         <v>8</v>
       </c>
@@ -3846,7 +3846,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A92">
         <v>8</v>
       </c>
@@ -3881,7 +3881,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A93">
         <v>8</v>
       </c>
@@ -3916,7 +3916,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A94">
         <v>8</v>
       </c>
@@ -3951,7 +3951,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A95">
         <v>8</v>
       </c>
@@ -3986,7 +3986,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A96">
         <v>8</v>
       </c>
@@ -4021,7 +4021,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="97" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A97">
         <v>8</v>
       </c>
@@ -4050,7 +4050,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="98" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A98">
         <v>8</v>
       </c>
@@ -4085,7 +4085,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="99" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A99">
         <v>9</v>
       </c>
@@ -4120,7 +4120,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="100" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="100" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A100">
         <v>9</v>
       </c>
@@ -4155,7 +4155,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="101" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="101" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A101">
         <v>9</v>
       </c>
@@ -4190,7 +4190,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="102" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="102" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A102">
         <v>9</v>
       </c>
@@ -4225,7 +4225,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="103" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="103" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A103">
         <v>9</v>
       </c>
@@ -4260,7 +4260,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="104" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="104" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A104">
         <v>9</v>
       </c>
@@ -4295,7 +4295,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="105" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="105" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A105">
         <v>9</v>
       </c>
@@ -4330,7 +4330,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="106" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="106" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A106">
         <v>9</v>
       </c>
@@ -4365,7 +4365,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="107" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="107" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A107">
         <v>9</v>
       </c>
@@ -4400,7 +4400,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="108" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="108" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A108">
         <v>9</v>
       </c>
@@ -4435,7 +4435,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="109" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="109" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A109">
         <v>9</v>
       </c>
@@ -4470,7 +4470,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="110" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="110" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A110">
         <v>9</v>
       </c>
@@ -4505,7 +4505,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="111" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="111" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A111">
         <v>9</v>
       </c>
@@ -4540,7 +4540,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="112" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="112" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A112">
         <v>10</v>
       </c>
@@ -4575,7 +4575,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="113" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="113" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A113">
         <v>10</v>
       </c>
@@ -4610,7 +4610,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="114" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="114" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A114">
         <v>10</v>
       </c>
@@ -4645,7 +4645,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="115" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="115" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A115">
         <v>10</v>
       </c>
@@ -4680,7 +4680,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="116" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="116" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A116">
         <v>10</v>
       </c>
@@ -4715,7 +4715,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="117" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="117" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A117">
         <v>10</v>
       </c>
@@ -4747,7 +4747,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="118" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="118" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A118">
         <v>10</v>
       </c>
@@ -4782,7 +4782,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="119" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="119" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A119">
         <v>10</v>
       </c>
@@ -4817,7 +4817,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="120" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="120" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A120">
         <v>10</v>
       </c>
@@ -4852,7 +4852,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="121" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="121" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A121">
         <v>10</v>
       </c>
@@ -4887,7 +4887,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="122" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="122" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A122">
         <v>10</v>
       </c>
@@ -4922,7 +4922,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="123" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="123" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A123">
         <v>10</v>
       </c>
@@ -4957,7 +4957,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="124" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="124" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A124">
         <v>10</v>
       </c>
@@ -4992,7 +4992,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="125" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="125" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A125">
         <v>10</v>
       </c>
@@ -5027,7 +5027,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="126" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="126" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A126">
         <v>10</v>
       </c>
@@ -5062,7 +5062,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="127" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="127" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A127">
         <v>11</v>
       </c>
@@ -5097,7 +5097,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="128" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="128" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A128">
         <v>11</v>
       </c>
@@ -5132,7 +5132,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="129" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="129" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A129">
         <v>11</v>
       </c>
@@ -5167,7 +5167,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="130" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="130" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A130">
         <v>11</v>
       </c>
@@ -5202,7 +5202,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="131" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="131" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A131">
         <v>11</v>
       </c>
@@ -5237,7 +5237,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="132" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="132" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A132">
         <v>11</v>
       </c>
@@ -5272,7 +5272,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="133" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="133" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A133">
         <v>11</v>
       </c>
@@ -5307,7 +5307,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="134" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="134" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A134">
         <v>11</v>
       </c>
@@ -5342,7 +5342,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="135" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="135" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A135">
         <v>11</v>
       </c>
@@ -5377,7 +5377,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="136" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="136" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A136">
         <v>11</v>
       </c>
@@ -5412,7 +5412,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="137" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="137" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A137">
         <v>11</v>
       </c>
@@ -5447,7 +5447,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="138" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="138" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A138">
         <v>11</v>
       </c>
@@ -5482,7 +5482,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="139" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="139" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A139">
         <v>11</v>
       </c>
@@ -5517,7 +5517,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="140" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="140" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A140">
         <v>12</v>
       </c>
@@ -5552,7 +5552,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="141" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="141" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A141">
         <v>12</v>
       </c>
@@ -5587,7 +5587,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="142" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="142" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A142">
         <v>12</v>
       </c>
@@ -5622,7 +5622,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="143" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="143" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A143">
         <v>12</v>
       </c>
@@ -5657,7 +5657,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="144" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="144" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A144">
         <v>12</v>
       </c>
@@ -5692,7 +5692,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="145" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="145" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A145">
         <v>12</v>
       </c>
@@ -5727,7 +5727,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="146" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="146" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A146">
         <v>12</v>
       </c>
@@ -5762,7 +5762,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="147" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="147" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A147">
         <v>12</v>
       </c>
@@ -5797,7 +5797,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="148" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="148" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A148">
         <v>12</v>
       </c>
@@ -5832,7 +5832,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="149" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="149" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A149">
         <v>12</v>
       </c>
@@ -5867,7 +5867,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="150" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="150" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A150">
         <v>12</v>
       </c>
@@ -5902,7 +5902,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="151" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="151" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A151">
         <v>12</v>
       </c>
@@ -5937,7 +5937,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="152" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="152" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A152">
         <v>12</v>
       </c>
@@ -5972,7 +5972,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="153" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="153" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A153">
         <v>12</v>
       </c>
@@ -6007,7 +6007,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="154" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="154" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A154">
         <v>12</v>
       </c>
@@ -6042,7 +6042,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="155" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="155" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A155">
         <v>13</v>
       </c>
@@ -6074,7 +6074,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="156" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="156" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A156">
         <v>13</v>
       </c>
@@ -6106,7 +6106,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="157" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="157" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A157">
         <v>13</v>
       </c>
@@ -6138,7 +6138,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="158" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="158" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A158">
         <v>13</v>
       </c>
@@ -6170,7 +6170,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="159" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="159" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A159">
         <v>13</v>
       </c>
@@ -6202,7 +6202,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="160" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="160" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A160">
         <v>13</v>
       </c>
@@ -6234,7 +6234,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="161" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="161" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A161">
         <v>13</v>
       </c>
@@ -6266,7 +6266,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="162" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="162" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A162">
         <v>13</v>
       </c>
@@ -6298,7 +6298,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="163" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="163" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A163">
         <v>13</v>
       </c>
@@ -6330,7 +6330,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="164" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="164" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A164">
         <v>13</v>
       </c>
@@ -6362,7 +6362,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="165" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="165" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A165">
         <v>13</v>
       </c>
@@ -6394,7 +6394,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="166" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="166" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A166">
         <v>13</v>
       </c>
@@ -6426,7 +6426,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="167" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="167" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A167">
         <v>13</v>
       </c>
@@ -6458,7 +6458,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="168" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="168" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A168">
         <v>13</v>
       </c>
@@ -6490,7 +6490,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="169" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="169" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A169">
         <v>14</v>
       </c>
@@ -6522,7 +6522,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="170" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="170" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A170">
         <v>14</v>
       </c>
@@ -6554,7 +6554,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="171" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="171" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A171">
         <v>14</v>
       </c>
@@ -6586,7 +6586,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="172" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="172" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A172">
         <v>14</v>
       </c>
@@ -6618,7 +6618,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="173" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="173" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A173">
         <v>14</v>
       </c>
@@ -6650,7 +6650,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="174" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="174" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A174">
         <v>14</v>
       </c>
@@ -6682,7 +6682,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="175" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="175" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A175">
         <v>14</v>
       </c>
@@ -6714,7 +6714,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="176" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="176" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A176">
         <v>14</v>
       </c>
@@ -6746,7 +6746,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="177" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="177" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A177">
         <v>14</v>
       </c>
@@ -6778,7 +6778,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="178" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="178" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A178">
         <v>14</v>
       </c>
@@ -6810,7 +6810,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="179" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="179" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A179">
         <v>14</v>
       </c>
@@ -6842,7 +6842,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="180" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="180" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A180">
         <v>14</v>
       </c>
@@ -6874,7 +6874,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="181" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="181" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A181">
         <v>14</v>
       </c>
@@ -6906,7 +6906,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="182" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="182" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A182">
         <v>14</v>
       </c>
@@ -6938,7 +6938,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="183" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="183" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A183">
         <v>15</v>
       </c>
@@ -6970,7 +6970,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="184" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="184" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A184">
         <v>15</v>
       </c>
@@ -7002,7 +7002,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="185" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="185" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A185">
         <v>15</v>
       </c>
@@ -7034,7 +7034,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="186" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="186" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A186">
         <v>15</v>
       </c>
@@ -7066,7 +7066,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="187" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="187" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A187">
         <v>15</v>
       </c>
@@ -7098,7 +7098,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="188" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="188" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A188">
         <v>15</v>
       </c>
@@ -7130,7 +7130,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="189" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="189" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A189">
         <v>15</v>
       </c>
@@ -7162,7 +7162,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="190" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="190" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A190">
         <v>15</v>
       </c>
@@ -7191,7 +7191,7 @@
         <v>0.56999999999999995</v>
       </c>
     </row>
-    <row r="191" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="191" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A191">
         <v>15</v>
       </c>
@@ -7223,7 +7223,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="192" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="192" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A192">
         <v>15</v>
       </c>
@@ -7255,7 +7255,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="193" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="193" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A193">
         <v>15</v>
       </c>
@@ -7287,7 +7287,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="194" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="194" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A194">
         <v>15</v>
       </c>
@@ -7319,7 +7319,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="195" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="195" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A195">
         <v>15</v>
       </c>
@@ -7351,7 +7351,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="196" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="196" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A196">
         <v>15</v>
       </c>
@@ -7383,7 +7383,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="197" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="197" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A197">
         <v>16</v>
       </c>
@@ -7415,7 +7415,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="198" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="198" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A198">
         <v>16</v>
       </c>
@@ -7447,7 +7447,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="199" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="199" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A199">
         <v>16</v>
       </c>
@@ -7479,7 +7479,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="200" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="200" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A200">
         <v>16</v>
       </c>
@@ -7511,7 +7511,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="201" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="201" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A201">
         <v>16</v>
       </c>
@@ -7543,7 +7543,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="202" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="202" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A202">
         <v>16</v>
       </c>
@@ -7575,7 +7575,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="203" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="203" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A203">
         <v>16</v>
       </c>
@@ -7607,7 +7607,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="204" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="204" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A204">
         <v>16</v>
       </c>
@@ -7639,7 +7639,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="205" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="205" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A205">
         <v>16</v>
       </c>
@@ -7671,7 +7671,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="206" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="206" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A206">
         <v>16</v>
       </c>
@@ -7703,7 +7703,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="207" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="207" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A207">
         <v>16</v>
       </c>
@@ -7735,7 +7735,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="208" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="208" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A208">
         <v>16</v>
       </c>
@@ -7767,7 +7767,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="209" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="209" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A209">
         <v>16</v>
       </c>
@@ -7799,7 +7799,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="210" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="210" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A210">
         <v>16</v>
       </c>
@@ -7831,7 +7831,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="211" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="211" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A211">
         <v>17</v>
       </c>
@@ -7863,7 +7863,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="212" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="212" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A212">
         <v>17</v>
       </c>
@@ -7895,7 +7895,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="213" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="213" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A213">
         <v>17</v>
       </c>
@@ -7927,7 +7927,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="214" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="214" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A214">
         <v>17</v>
       </c>
@@ -7956,7 +7956,7 @@
         <v>1.84</v>
       </c>
     </row>
-    <row r="215" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="215" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A215">
         <v>17</v>
       </c>
@@ -7988,7 +7988,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="216" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="216" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A216">
         <v>17</v>
       </c>
@@ -8020,7 +8020,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="217" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="217" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A217">
         <v>17</v>
       </c>
@@ -8049,7 +8049,7 @@
         <v>0.53</v>
       </c>
     </row>
-    <row r="218" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="218" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A218">
         <v>17</v>
       </c>
@@ -8081,7 +8081,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="219" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="219" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A219">
         <v>17</v>
       </c>
@@ -8113,7 +8113,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="220" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="220" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A220">
         <v>17</v>
       </c>
@@ -8145,7 +8145,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="221" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="221" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A221">
         <v>17</v>
       </c>
@@ -8177,7 +8177,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="222" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="222" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A222">
         <v>17</v>
       </c>
@@ -8209,7 +8209,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="223" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="223" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A223">
         <v>17</v>
       </c>
@@ -8241,7 +8241,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="224" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="224" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A224">
         <v>17</v>
       </c>
@@ -8273,7 +8273,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="225" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="225" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A225">
         <v>18</v>
       </c>
@@ -8305,7 +8305,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="226" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="226" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A226">
         <v>18</v>
       </c>
@@ -8337,7 +8337,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="227" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="227" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A227">
         <v>18</v>
       </c>
@@ -8369,7 +8369,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="228" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="228" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A228">
         <v>18</v>
       </c>
@@ -8401,7 +8401,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="229" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="229" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A229">
         <v>18</v>
       </c>
@@ -8433,7 +8433,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="230" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="230" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A230">
         <v>18</v>
       </c>
@@ -8465,7 +8465,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="231" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="231" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A231">
         <v>18</v>
       </c>
@@ -8497,7 +8497,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="232" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="232" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A232">
         <v>18</v>
       </c>
@@ -8529,7 +8529,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="233" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="233" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A233">
         <v>18</v>
       </c>
@@ -8558,7 +8558,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="234" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="234" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A234">
         <v>18</v>
       </c>
@@ -8590,7 +8590,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="235" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="235" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A235">
         <v>18</v>
       </c>
@@ -8622,7 +8622,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="236" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="236" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A236">
         <v>18</v>
       </c>
@@ -8654,7 +8654,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="237" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="237" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A237">
         <v>18</v>
       </c>
@@ -8686,7 +8686,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="238" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="238" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A238">
         <v>18</v>
       </c>
@@ -8718,7 +8718,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="239" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="239" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A239">
         <v>19</v>
       </c>
@@ -8750,7 +8750,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="240" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="240" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A240">
         <v>19</v>
       </c>
@@ -8782,7 +8782,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="241" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="241" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A241">
         <v>19</v>
       </c>
@@ -8814,7 +8814,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="242" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="242" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A242">
         <v>19</v>
       </c>
@@ -8846,7 +8846,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="243" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="243" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A243">
         <v>19</v>
       </c>
@@ -8878,7 +8878,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="244" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="244" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A244">
         <v>19</v>
       </c>
@@ -8910,7 +8910,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="245" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="245" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A245">
         <v>19</v>
       </c>
@@ -8942,7 +8942,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="246" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="246" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A246">
         <v>19</v>
       </c>
@@ -8974,7 +8974,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="247" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="247" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A247">
         <v>19</v>
       </c>
@@ -9006,7 +9006,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="248" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="248" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A248">
         <v>19</v>
       </c>
@@ -9038,7 +9038,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="249" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="249" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A249">
         <v>19</v>
       </c>
@@ -9070,7 +9070,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="250" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="250" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A250">
         <v>19</v>
       </c>
@@ -9102,7 +9102,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="251" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="251" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A251">
         <v>19</v>
       </c>
@@ -9134,7 +9134,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="252" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="252" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A252">
         <v>19</v>
       </c>
@@ -9166,7 +9166,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="253" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="253" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A253">
         <v>20</v>
       </c>
@@ -9200,7 +9200,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="254" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="254" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A254">
         <v>20</v>
       </c>
@@ -9234,7 +9234,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="255" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="255" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A255">
         <v>20</v>
       </c>
@@ -9268,7 +9268,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="256" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="256" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A256">
         <v>20</v>
       </c>
@@ -9302,7 +9302,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="257" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="257" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A257">
         <v>20</v>
       </c>
@@ -9336,7 +9336,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="258" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="258" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A258">
         <v>20</v>
       </c>
@@ -9370,7 +9370,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="259" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="259" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A259">
         <v>20</v>
       </c>
@@ -9404,7 +9404,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="260" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="260" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A260">
         <v>20</v>
       </c>
@@ -9437,7 +9437,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="261" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="261" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A261">
         <v>20</v>
       </c>
@@ -9471,7 +9471,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="262" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="262" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A262">
         <v>20</v>
       </c>
@@ -9505,7 +9505,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="263" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="263" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A263">
         <v>20</v>
       </c>
@@ -9539,7 +9539,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="264" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="264" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A264">
         <v>20</v>
       </c>
@@ -9573,7 +9573,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="265" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="265" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A265">
         <v>20</v>
       </c>
@@ -9607,7 +9607,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="266" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="266" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A266">
         <v>20</v>
       </c>
@@ -9641,7 +9641,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="267" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="267" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A267">
         <v>21</v>
       </c>
@@ -9675,7 +9675,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="268" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="268" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A268">
         <v>21</v>
       </c>
@@ -9709,7 +9709,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="269" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="269" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A269">
         <v>21</v>
       </c>
@@ -9743,7 +9743,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="270" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="270" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A270">
         <v>21</v>
       </c>
@@ -9777,7 +9777,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="271" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="271" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A271">
         <v>21</v>
       </c>
@@ -9811,7 +9811,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="272" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="272" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A272">
         <v>21</v>
       </c>
@@ -9845,7 +9845,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="273" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="273" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A273">
         <v>21</v>
       </c>
@@ -9879,7 +9879,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="274" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="274" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A274">
         <v>21</v>
       </c>
@@ -9913,7 +9913,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="275" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="275" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A275">
         <v>21</v>
       </c>
@@ -9947,7 +9947,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="276" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="276" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A276">
         <v>21</v>
       </c>
@@ -9981,7 +9981,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="277" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="277" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A277">
         <v>21</v>
       </c>
@@ -10015,7 +10015,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="278" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="278" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A278">
         <v>21</v>
       </c>
@@ -10049,7 +10049,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="279" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="279" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A279">
         <v>21</v>
       </c>
@@ -10083,7 +10083,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="280" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="280" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A280">
         <v>21</v>
       </c>

</xml_diff>